<commit_message>
Mídias + Imagens + Diagrama
</commit_message>
<xml_diff>
--- a/ResultadosGerais/Diagrama_GEOs_AGEOs.xlsx
+++ b/ResultadosGerais/Diagrama_GEOs_AGEOs.xlsx
@@ -69,7 +69,7 @@
     <t>Alteração do valor de τ  (AGEOs)</t>
   </si>
   <si>
-    <t>Rankeamento e Mutação</t>
+    <t>Ranqueamento e Mutação</t>
   </si>
   <si>
     <t>Verificação do Critério de Parada</t>
@@ -116,10 +116,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -177,7 +177,84 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,6 +268,14 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -198,100 +283,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,6 +304,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -321,19 +321,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,25 +363,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +411,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,43 +435,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,7 +447,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,19 +495,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,32 +505,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="68">
+  <borders count="69">
     <border>
       <left/>
       <right/>
@@ -831,6 +831,19 @@
       <top/>
       <bottom style="thin">
         <color auto="true"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1266,15 +1279,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1320,17 +1324,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1349,8 +1342,19 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1359,7 +1363,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1368,142 +1381,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="68" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="66" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="66" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="64" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="65" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="64" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="63" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="61" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="61" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="61" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="61" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="67" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="65" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="60" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="60" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="67" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="62" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="62" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1513,7 +1526,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1625,64 +1638,67 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true" applyAlignment="true">
@@ -1697,11 +1713,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
@@ -1709,23 +1725,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="true">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="true">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
@@ -1739,6 +1755,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
@@ -1748,25 +1767,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -8305,7 +8324,7 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 52413"/>
+            <a:gd name="adj1" fmla="val 53987"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -9176,9 +9195,7 @@
         </a:prstGeom>
         <a:ln w="38100">
           <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow" w="med" len="med"/>
         </a:ln>
@@ -9203,29 +9220,32 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1960245</xdr:colOff>
+      <xdr:colOff>1946910</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>835660</xdr:rowOff>
+      <xdr:rowOff>835025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>52070</xdr:colOff>
+      <xdr:colOff>38735</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>798830</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="29" name="Elbow Connector 28"/>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="3"/>
+          <a:endCxn id="26" idx="3"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true">
-          <a:off x="12815570" y="6830060"/>
-          <a:ext cx="419100" cy="1639570"/>
+          <a:off x="12802235" y="6829425"/>
+          <a:ext cx="419100" cy="1640205"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -147799"/>
+            <a:gd name="adj1" fmla="val -153484"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -9467,9 +9487,7 @@
         </a:prstGeom>
         <a:ln w="38100">
           <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow" w="med" len="med"/>
         </a:ln>
@@ -9767,7 +9785,7 @@
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
               <a:sym typeface="+mn-ea"/>
             </a:rPr>
-            <a:t> de acordo com o fitness </a:t>
+            <a:t> de acordo com o valor da função </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
@@ -9999,7 +10017,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
-            <a:t>de acordo com o fitness e muta 1 bit </a:t>
+            <a:t>de acordo com o valor da função e muta 1 bit </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600" b="1"/>
@@ -10014,15 +10032,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
+      <xdr:colOff>802005</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>216535</xdr:rowOff>
+      <xdr:rowOff>349885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1707515</xdr:colOff>
+      <xdr:colOff>1718945</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1811655</xdr:rowOff>
+      <xdr:rowOff>1945005</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10031,7 +10049,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6983730" y="12840335"/>
+          <a:off x="6995160" y="12973685"/>
           <a:ext cx="3251835" cy="1595120"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -10173,15 +10191,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>305435</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>217805</xdr:rowOff>
+      <xdr:rowOff>216535</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1972310</xdr:colOff>
+      <xdr:colOff>1990725</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1123315</xdr:rowOff>
+      <xdr:rowOff>1122045</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10190,7 +10208,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2043430" y="14962505"/>
+          <a:off x="2061845" y="14961235"/>
           <a:ext cx="13111480" cy="905510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -10321,7 +10339,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
-            <a:t>Retorna a melhor solução durante a execução</a:t>
+            <a:t>Retorna a melhor solução obtida durante a busca</a:t>
           </a:r>
           <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600"/>
         </a:p>
@@ -10332,15 +10350,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>70485</xdr:colOff>
+      <xdr:colOff>92710</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1811020</xdr:rowOff>
+      <xdr:rowOff>1944370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>78740</xdr:colOff>
+      <xdr:colOff>94615</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>217805</xdr:rowOff>
+      <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -10352,8 +10370,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true">
-          <a:off x="8598535" y="14434820"/>
-          <a:ext cx="8255" cy="527685"/>
+          <a:off x="8620760" y="14568170"/>
+          <a:ext cx="1905" cy="392430"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10552,7 +10570,7 @@
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
               <a:sym typeface="+mn-ea"/>
             </a:rPr>
-            <a:t>de acordo com o fitness e muta 1 bit </a:t>
+            <a:t>de acordo com o valor da função e muta 1 bit </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600" b="1">
@@ -10736,7 +10754,7 @@
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
               <a:sym typeface="+mn-ea"/>
             </a:rPr>
-            <a:t> de acordo com o fitness e muta 1 bit </a:t>
+            <a:t> de acordo com o valor da função e muta 1 bit </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600" b="1">
@@ -10756,64 +10774,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1070610</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1094105</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>513080</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1095375</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>212090</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="42" name="Straight Arrow Connector 41"/>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="41" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7263765" y="9733280"/>
-          <a:ext cx="24765" cy="372110"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1084580</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>499110</xdr:rowOff>
+      <xdr:rowOff>497840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -10828,8 +10792,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9612630" y="9719310"/>
-          <a:ext cx="11430" cy="385445"/>
+          <a:off x="9622155" y="9718040"/>
+          <a:ext cx="1905" cy="386715"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -11233,7 +11197,7 @@
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
               <a:sym typeface="+mn-ea"/>
             </a:rPr>
-            <a:t> de acordo com o fitness e muta 1 bit </a:t>
+            <a:t> de acordo com o valor da função e muta 1 bit </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600" b="1">
@@ -11254,9 +11218,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1084580</xdr:colOff>
+      <xdr:colOff>1094740</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>499110</xdr:rowOff>
+      <xdr:rowOff>497840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -11271,8 +11235,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11939905" y="9719310"/>
-          <a:ext cx="11430" cy="385445"/>
+          <a:off x="11950065" y="9718040"/>
+          <a:ext cx="1270" cy="386715"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -11456,15 +11420,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1707515</xdr:colOff>
+      <xdr:colOff>1718310</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>647065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2162175</xdr:colOff>
+      <xdr:colOff>2162810</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1013460</xdr:rowOff>
+      <xdr:rowOff>1146810</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -11476,12 +11440,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="true">
-          <a:off x="10235565" y="3390265"/>
-          <a:ext cx="5109210" cy="10246995"/>
+          <a:off x="10246360" y="3390265"/>
+          <a:ext cx="5099050" cy="10380345"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 104661"/>
+            <a:gd name="adj1" fmla="val 104664"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -11678,7 +11642,7 @@
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
               <a:sym typeface="+mn-ea"/>
             </a:rPr>
-            <a:t>de acordo com o fitness e muta 1 bit </a:t>
+            <a:t>de acordo com o valor da funçãoe muta 1 bit </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-PT" altLang="en-US" sz="1600" b="1">
@@ -11695,13 +11659,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1084580</xdr:colOff>
+      <xdr:colOff>1094105</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>499110</xdr:rowOff>
+      <xdr:rowOff>497840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1096010</xdr:colOff>
+      <xdr:colOff>1094740</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>211455</xdr:rowOff>
     </xdr:to>
@@ -11712,8 +11676,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14267180" y="9719310"/>
-          <a:ext cx="11430" cy="385445"/>
+          <a:off x="14276705" y="9718040"/>
+          <a:ext cx="635" cy="386715"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -11770,7 +11734,7 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 49926"/>
+            <a:gd name="adj1" fmla="val 50143"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -11800,32 +11764,29 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1642745</xdr:colOff>
+      <xdr:colOff>1625600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1877695</xdr:rowOff>
+      <xdr:rowOff>1876425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1166495</xdr:colOff>
+      <xdr:colOff>1149350</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>173990</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="59" name="Elbow Connector 58"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="18" idx="2"/>
-          <a:endCxn id="21" idx="0"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="8543290" y="5018405"/>
+          <a:off x="8526145" y="5017135"/>
           <a:ext cx="443865" cy="1858645"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj1" fmla="val 50286"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -11955,15 +11916,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1042035</xdr:colOff>
+      <xdr:colOff>1041082</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1008380</xdr:rowOff>
+      <xdr:rowOff>1007427</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>78740</xdr:colOff>
+      <xdr:colOff>94297</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
+      <xdr:rowOff>348932</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -11975,8 +11936,228 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipV="true">
-          <a:off x="5473700" y="9706610"/>
-          <a:ext cx="439420" cy="5826760"/>
+          <a:off x="5413375" y="9763760"/>
+          <a:ext cx="573405" cy="5843270"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50056"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1108392</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>978852</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>94297</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>348297</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Elbow Connector 78"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="34" idx="2"/>
+          <a:endCxn id="37" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipV="true">
+          <a:off x="6530340" y="10880090"/>
+          <a:ext cx="601345" cy="3581400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50370"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>993775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>94615</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Elbow Connector 79"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="41" idx="2"/>
+          <a:endCxn id="37" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipV="true">
+          <a:off x="7661910" y="12012295"/>
+          <a:ext cx="587375" cy="1334135"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50055"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>94615</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>993775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1040130</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>349250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Elbow Connector 80"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="2"/>
+          <a:endCxn id="37" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8801735" y="12206605"/>
+          <a:ext cx="587375" cy="945515"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50055"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>94297</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>993457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1039812</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>348932</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="82" name="Elbow Connector 81"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="49" idx="2"/>
+          <a:endCxn id="37" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="9964420" y="11042015"/>
+          <a:ext cx="587375" cy="3272790"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -12009,247 +12190,33 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>94297</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>979805</xdr:rowOff>
+      <xdr:rowOff>992822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1040447</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>215265</xdr:rowOff>
+      <xdr:rowOff>348297</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="Elbow Connector 78"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000" flipV="true">
-          <a:off x="6578600" y="10822940"/>
-          <a:ext cx="467360" cy="3564890"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 52500"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1095375</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>994410</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>78740</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="80" name="Elbow Connector 79"/>
+        <xdr:cNvPr id="83" name="Elbow Connector 82"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="41" idx="2"/>
-          <a:endCxn id="37" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000" flipV="true">
-          <a:off x="7720965" y="11953875"/>
-          <a:ext cx="453390" cy="1318260"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50071"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>78422</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>994092</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1040447</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>215582</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="81" name="Elbow Connector 80"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="40" idx="2"/>
+          <a:stCxn id="56" idx="2"/>
           <a:endCxn id="37" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="8860155" y="12131040"/>
-          <a:ext cx="453390" cy="962025"/>
+          <a:off x="11128375" y="9877425"/>
+          <a:ext cx="587375" cy="5600700"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50071"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>78740</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>994410</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1040765</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="82" name="Elbow Connector 81"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="49" idx="2"/>
-          <a:endCxn id="37" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="10024745" y="10968355"/>
-          <a:ext cx="453390" cy="3289300"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50071"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>78105</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>993140</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1039495</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>214630</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="83" name="Elbow Connector 82"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="11187430" y="9803765"/>
-          <a:ext cx="453390" cy="5615940"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50071"/>
+            <a:gd name="adj1" fmla="val 49729"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -12913,109 +12880,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1632585</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1478280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1637665</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>142240</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Straight Arrow Connector 17"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7825740" y="7472680"/>
-          <a:ext cx="5080" cy="340360"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1629410</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1438275</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1637665</xdr:colOff>
+      <xdr:colOff>1085850</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>124460</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="Straight Arrow Connector 18"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="true">
-          <a:off x="7822565" y="9109075"/>
-          <a:ext cx="8255" cy="235585"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1061085</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>512445</xdr:rowOff>
+      <xdr:rowOff>489585</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -13030,8 +12897,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7254240" y="9732645"/>
-          <a:ext cx="24765" cy="372110"/>
+          <a:off x="7279005" y="9709785"/>
+          <a:ext cx="0" cy="394970"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -20418,110 +20285,110 @@
   </cols>
   <sheetData>
     <row r="1" ht="38" customHeight="true" spans="1:5">
-      <c r="A1" s="54"/>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="56"/>
+      <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="57" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="87" customHeight="true" spans="1:6">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="79"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="81"/>
     </row>
     <row r="3" ht="91" customHeight="true" spans="1:5">
-      <c r="A3" s="55"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="80"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="82"/>
     </row>
     <row r="4" ht="97" customHeight="true" spans="1:6">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="79"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="81"/>
     </row>
     <row r="5" ht="169" customHeight="true" spans="1:6">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="71"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="73"/>
     </row>
     <row r="6" ht="132" customHeight="true" spans="1:6">
-      <c r="A6" s="69"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="72"/>
-      <c r="F6" s="71"/>
+      <c r="A6" s="71"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="74"/>
+      <c r="F6" s="73"/>
     </row>
     <row r="7" ht="122" customHeight="true" spans="1:5">
-      <c r="A7" s="69"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="82" t="s">
+      <c r="A7" s="71"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="84" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" ht="53" customHeight="true" spans="1:6">
-      <c r="A8" s="69"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="75"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="79"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="81"/>
     </row>
     <row r="9" ht="118" customHeight="true" spans="1:4">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="77"/>
+      <c r="D9" s="79"/>
     </row>
     <row r="10" ht="97" customHeight="true" spans="1:6">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="72"/>
-      <c r="F10" s="79"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="74"/>
+      <c r="F10" s="81"/>
     </row>
     <row r="11" ht="149" customHeight="true" spans="1:4">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="D11" s="77"/>
+      <c r="B11" s="74"/>
+      <c r="D11" s="79"/>
     </row>
     <row r="12" ht="105" customHeight="true" spans="1:6">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="84"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -20537,13 +20404,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I13" sqref="A1:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="22.8083333333333" customWidth="true"/>
     <col min="2" max="2" width="28.8" customWidth="true"/>
@@ -20570,10 +20437,10 @@
       <c r="F1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="38"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" ht="87" customHeight="true" spans="1:8">
       <c r="A2" s="18" t="s">
@@ -20584,8 +20451,8 @@
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" ht="91" customHeight="true" spans="1:8">
       <c r="A3" s="18"/>
@@ -20594,8 +20461,8 @@
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" ht="87" customHeight="true" spans="1:8">
       <c r="A4" s="23" t="s">
@@ -20606,8 +20473,8 @@
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="45"/>
     </row>
     <row r="5" ht="169" customHeight="true" spans="1:8">
       <c r="A5" s="18" t="s">
@@ -20618,8 +20485,8 @@
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="40"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" ht="132" customHeight="true" spans="1:8">
       <c r="A6" s="18"/>
@@ -20628,8 +20495,8 @@
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" ht="122" customHeight="true" spans="1:8">
       <c r="A7" s="18"/>
@@ -20638,8 +20505,8 @@
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="47"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" ht="53" customHeight="true" spans="1:8">
       <c r="A8" s="18"/>
@@ -20648,8 +20515,8 @@
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="42"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="9" ht="118" customHeight="true" spans="1:8">
       <c r="A9" s="18" t="s">
@@ -20660,8 +20527,8 @@
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="40"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" ht="97" customHeight="true" spans="1:8">
       <c r="A10" s="18"/>
@@ -20670,8 +20537,8 @@
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="42"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="43"/>
     </row>
     <row r="11" ht="167" customHeight="true" spans="1:8">
       <c r="A11" s="18" t="s">
@@ -20682,8 +20549,8 @@
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="52"/>
     </row>
     <row r="12" ht="105" customHeight="true" spans="1:8">
       <c r="A12" s="34" t="s">
@@ -20694,8 +20561,19 @@
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="54"/>
+    </row>
+    <row r="13" ht="42" customHeight="true" spans="1:9">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
[WIP] Arquivos e Execuções
</commit_message>
<xml_diff>
--- a/ResultadosGerais/Diagrama_GEOs_AGEOs.xlsx
+++ b/ResultadosGerais/Diagrama_GEOs_AGEOs.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19665" windowHeight="7980"/>
+    <workbookView windowWidth="14460" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DiagramaREAL" sheetId="5" r:id="rId1"/>
-    <sheet name="DiagramaBINARIO" sheetId="6" r:id="rId2"/>
-    <sheet name="Funções" sheetId="4" r:id="rId3"/>
+    <sheet name="DiagramaREAL_basic" sheetId="5" r:id="rId1"/>
+    <sheet name="DiagramaBIN_basic" sheetId="7" r:id="rId2"/>
+    <sheet name="DiagramaBINARIO" sheetId="6" r:id="rId3"/>
+    <sheet name="Funções" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>GEOreal1</t>
   </si>
@@ -27,7 +28,7 @@
     <t>Inicialização</t>
   </si>
   <si>
-    <t>Verificação de f(x) ao mutar</t>
+    <t>Verificação de f(x) ao perturbar</t>
   </si>
   <si>
     <t>Ranqueamento e Mutação</t>
@@ -39,10 +40,13 @@
     <t>Obtenção do Resultado Final</t>
   </si>
   <si>
+    <t>GEO</t>
+  </si>
+  <si>
     <t>GEOvar</t>
   </si>
   <si>
-    <t>GEO</t>
+    <t>Verificação de f(x) ao mutar</t>
   </si>
   <si>
     <t>A-GEO1</t>
@@ -99,9 +103,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -142,28 +146,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -172,70 +154,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -258,15 +179,67 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,8 +252,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,49 +299,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,19 +329,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,49 +353,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,19 +371,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,13 +407,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,6 +1025,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1031,32 +1059,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1079,32 +1081,34 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1113,121 +1117,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="48" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="47" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="47" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="42" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="45" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="42" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="44" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="42" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="44" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1236,25 +1240,25 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="43" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="48" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3670,7 +3674,7 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50081"/>
+            <a:gd name="adj1" fmla="val 28548"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -3725,7 +3729,7 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50070"/>
+            <a:gd name="adj1" fmla="val 37621"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -4251,7 +4255,7 @@
                           <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
                           <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑏𝑒𝑠𝑡</m:t>
+                        <m:t>𝑏𝑠𝑡</m:t>
                       </m:r>
                     </m:sub>
                   </m:sSub>
@@ -4695,7 +4699,7 @@
                   <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
                   <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
                 </a:rPr>
-                <a:t>𝑏𝑒𝑠𝑡</a:t>
+                <a:t>𝑏𝑠𝑡</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
@@ -6696,6 +6700,3439 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2719705</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1931670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3226435</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2124075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Text Box 1"/>
+        <xdr:cNvSpPr txBox="true"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4457700" y="10034270"/>
+          <a:ext cx="506730" cy="192405"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-PT" altLang="en-US" sz="1100" b="1">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t>Sim</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1100" b="1">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3629025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2313305</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>473075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2537460</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Text Box 2"/>
+        <xdr:cNvSpPr txBox="true"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5367020" y="10261600"/>
+          <a:ext cx="497840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-PT" altLang="en-US" sz="1100" b="1">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t>Sim</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1100" b="1">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1014730</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1207770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1597660</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1568450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Text Box 3"/>
+        <xdr:cNvSpPr txBox="true"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6406515" y="9310370"/>
+          <a:ext cx="582930" cy="360680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-PT" altLang="en-US" sz="1100" b="1">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t>Não</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1100" b="1">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>188595</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>170815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3463290</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>895985</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rounded Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1926590" y="488315"/>
+          <a:ext cx="6928485" cy="725170"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>Inicializa randomicamente a população de bits que codificam N variáveis de projeto</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>921385</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>913765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>924560</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>913765</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9755505" y="1231265"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>909320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>955675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>909320</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10396220" y="1226820"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1256665</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>899160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1259840</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>271780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648450" y="1216660"/>
+          <a:ext cx="3175" cy="477520"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1160145</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>911860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1163320</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>284480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2898140" y="1229360"/>
+          <a:ext cx="3175" cy="477520"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>921385</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>934085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>924560</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>934085</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="true">
+          <a:off x="9755505" y="2356485"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>946785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>955675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>946785</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="true">
+          <a:off x="10396220" y="2369185"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1824355</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3804285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1833245</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>249555</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3562350" y="5226685"/>
+          <a:ext cx="8890" cy="394970"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1731645</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3805555</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1736725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>226060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="true">
+          <a:off x="7123430" y="5227955"/>
+          <a:ext cx="5080" cy="370205"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>452755</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>262890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3154680</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1058545</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="Rounded Rectangle 13"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2190750" y="5634990"/>
+              <a:ext cx="2701925" cy="2294255"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="en-US">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t>Ranqueia os pares da população inteira de acordo com o </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑉</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t> e escolhe uma das perturbações para ocorrer com probabilidade proporcional a </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSubSup>
+                    <m:sSubSupPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubSupPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑘</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖</m:t>
+                      </m:r>
+                    </m:sub>
+                    <m:sup>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>−</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝜏</m:t>
+                      </m:r>
+                    </m:sup>
+                  </m:sSubSup>
+                </m:oMath>
+              </a14:m>
+              <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="Rounded Rectangle 13"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2190750" y="5634990"/>
+              <a:ext cx="2701925" cy="2294255"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="en-US">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t>Ranqueia os pares da população inteira de acordo com o </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t> e escolhe uma das perturbações para ocorrer com probabilidade proporcional a </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑘</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝜏</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2026285</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>995680</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1995170</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Diamond 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3764280" y="8331200"/>
+          <a:ext cx="2623185" cy="1766570"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+            <a:t>Critério de Parada atingido?</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>322580</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2687955</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1067435</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rounded Rectangle 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2060575" y="10423525"/>
+          <a:ext cx="6019165" cy="905510"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+            <a:t>Retorna a melhor solução obtida durante a busca</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3335655</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1994535</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3341370</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="2"/>
+          <a:endCxn id="16" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="true">
+          <a:off x="5073650" y="10097135"/>
+          <a:ext cx="5715" cy="326390"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>909320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>955675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>909320</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11106150" y="1226820"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>946785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>955675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>946785</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="true">
+          <a:off x="11106150" y="2369185"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>909320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>955675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>909320</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11816080" y="1226820"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>946785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>955675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>946785</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="true">
+          <a:off x="11816080" y="2369185"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1803717</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1058227</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3341052</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>227647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Elbow Connector 21"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="2"/>
+          <a:endCxn id="15" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipV="true">
+          <a:off x="4109085" y="7360285"/>
+          <a:ext cx="401320" cy="1537335"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28333"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3341370</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1000125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1654810</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>227965</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Elbow Connector 22"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="25" idx="2"/>
+          <a:endCxn id="15" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5833110" y="7117080"/>
+          <a:ext cx="459740" cy="1967230"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 37465"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>276860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3373120</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3771900</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="24" name="Rounded Rectangle 23"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2014220" y="1699260"/>
+              <a:ext cx="6750685" cy="3495040"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="en-US">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t>Muta cada bit da população e calcula o valor </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑉</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t> da função objetivo, gerando pares </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                      <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                    </a:rPr>
+                    <m:t>(</m:t>
+                  </m:r>
+                  <m:r>
+                    <m:rPr>
+                      <m:sty m:val="p"/>
+                    </m:rPr>
+                    <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                      <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                    </a:rPr>
+                    <m:t>i</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                      <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                    </a:rPr>
+                    <m:t>,</m:t>
+                  </m:r>
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑉</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                  <m:r>
+                    <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                      <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                      <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                    </a:rPr>
+                    <m:t>)</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t>. Se </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑉</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t> for melhor que  </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝐹</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑏𝑒𝑠𝑡</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>, a</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t>tualiza ele</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>.</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="24" name="Rounded Rectangle 23"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2014220" y="1699260"/>
+              <a:ext cx="6750685" cy="3495040"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="en-US">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t>Muta cada bit da população e calcula o valor </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t> da função objetivo, gerando pares </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>i</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t>. Se </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t> for melhor que  </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝐹</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑏𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>, a</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600"/>
+                <a:t>tualiza ele</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>.</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>205105</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3006090</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1000125</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="25" name="Rounded Rectangle 24"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5696585" y="5577205"/>
+              <a:ext cx="2701290" cy="2293620"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="en-US">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+                  <a:sym typeface="+mn-ea"/>
+                </a:rPr>
+                <a:t>Ranqueia os pares para cada variável de acordo com o </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑉</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+                  <a:sym typeface="+mn-ea"/>
+                </a:rPr>
+                <a:t> e escolhe uma das perturbações para ocorrer com probabilidade proporcional a </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSubSup>
+                    <m:sSubSupPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubSupPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑘</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑖</m:t>
+                      </m:r>
+                    </m:sub>
+                    <m:sup>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>−</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" altLang="pt-PT" sz="1600" i="1">
+                          <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                          <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝜏</m:t>
+                      </m:r>
+                    </m:sup>
+                  </m:sSubSup>
+                </m:oMath>
+              </a14:m>
+              <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600" b="1"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="25" name="Rounded Rectangle 24"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5696585" y="5577205"/>
+              <a:ext cx="2701290" cy="2293620"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent5"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent5"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="false"/>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="en-US">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+                  <a:sym typeface="+mn-ea"/>
+                </a:rPr>
+                <a:t>Ranqueia os pares para cada variável de acordo com o </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑉</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
+                  <a:sym typeface="+mn-ea"/>
+                </a:rPr>
+                <a:t> e escolhe uma das perturbações para ocorrer com probabilidade proporcional a </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑘</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
+                  <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                  <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
+                </a:rPr>
+                <a:t>𝜏</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600" b="1"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:endParaRPr lang="pt-PT" altLang="en-US" sz="1600" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1270</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>276860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>995045</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1111885</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Elbow Connector 26"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="3"/>
+          <a:endCxn id="24" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="true" flipV="true">
+          <a:off x="5393055" y="1699260"/>
+          <a:ext cx="993775" cy="7515225"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -261358"/>
+            <a:gd name="adj2" fmla="val 104807"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -13785,7 +17222,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -21125,8 +24562,8 @@
   <sheetPr/>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:C7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7"/>
@@ -21255,6 +24692,138 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7"/>
+  <cols>
+    <col min="1" max="1" width="22.8083333333333" customWidth="true"/>
+    <col min="2" max="2" width="47.95" customWidth="true"/>
+    <col min="3" max="3" width="48.8583333333333" customWidth="true"/>
+    <col min="4" max="5" width="8.40833333333333" customWidth="true"/>
+    <col min="6" max="7" width="9.31666666666667" customWidth="true"/>
+    <col min="8" max="8" width="8.85833333333333" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="true" spans="1:9">
+      <c r="A1" s="16"/>
+      <c r="B1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="65"/>
+    </row>
+    <row r="2" ht="87" customHeight="true" spans="1:9">
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+    </row>
+    <row r="3" ht="311" customHeight="true" spans="1:9">
+      <c r="A3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+    </row>
+    <row r="4" ht="118" customHeight="true" spans="1:9">
+      <c r="A4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+    </row>
+    <row r="5" ht="97" customHeight="true" spans="1:9">
+      <c r="A5" s="18"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+    </row>
+    <row r="6" ht="170" customHeight="true" spans="1:9">
+      <c r="A6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+    </row>
+    <row r="7" ht="93" customHeight="true" spans="1:9">
+      <c r="A7" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+    </row>
+    <row r="8" ht="42" customHeight="true" spans="1:9">
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -21274,22 +24843,22 @@
     <row r="1" ht="38" customHeight="true" spans="1:8">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" s="17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" s="39"/>
     </row>
@@ -21317,7 +24886,7 @@
     </row>
     <row r="4" ht="87" customHeight="true" spans="1:8">
       <c r="A4" s="23" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="25"/>
@@ -21329,7 +24898,7 @@
     </row>
     <row r="5" ht="169" customHeight="true" spans="1:8">
       <c r="A5" s="18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="27"/>
@@ -21439,7 +25008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="B1:I7"/>
@@ -21466,27 +25035,27 @@
     </row>
     <row r="2" ht="29.25" spans="2:7">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="40" customHeight="true" spans="2:7">
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5">
         <v>10</v>
@@ -21502,7 +25071,7 @@
     </row>
     <row r="4" ht="30" customHeight="true" spans="2:7">
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="8">
         <v>20</v>
@@ -21518,7 +25087,7 @@
     </row>
     <row r="5" ht="30" customHeight="true" spans="2:7">
       <c r="B5" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="8">
         <v>2</v>
@@ -21534,7 +25103,7 @@
     </row>
     <row r="6" ht="31" customHeight="true" spans="2:7">
       <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="8">
         <v>10</v>
@@ -21550,7 +25119,7 @@
     </row>
     <row r="7" ht="77" customHeight="true" spans="2:7">
       <c r="B7" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="11">
         <v>30</v>

</xml_diff>

<commit_message>
Tabelas + Slides + Imagens + Base pra chamada da spacecraft
</commit_message>
<xml_diff>
--- a/ResultadosGerais/Diagrama_GEOs_AGEOs.xlsx
+++ b/ResultadosGerais/Diagrama_GEOs_AGEOs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14460" windowHeight="7905" activeTab="1"/>
+    <workbookView windowWidth="19665" windowHeight="7905" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DiagramaREAL_basic" sheetId="5" r:id="rId1"/>
@@ -102,10 +102,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -146,17 +146,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,17 +156,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,6 +181,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,7 +209,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,8 +223,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,7 +233,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,14 +267,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -267,26 +274,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -299,7 +299,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,169 +473,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1015,11 +1015,56 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1041,39 +1086,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1089,26 +1106,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1117,148 +1117,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="47" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="47" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="42" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="45" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="44" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="44" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="42" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="44" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="48" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="43" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="48" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4255,7 +4255,7 @@
                           <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
                           <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑏𝑠𝑡</m:t>
+                        <m:t>𝑏𝑡</m:t>
                       </m:r>
                     </m:sub>
                   </m:sSub>
@@ -4699,7 +4699,7 @@
                   <a:latin typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
                   <a:cs typeface="DejaVu Math TeX Gyre" panose="02000503000000000000" charset="0"/>
                 </a:rPr>
-                <a:t>𝑏𝑠𝑡</a:t>
+                <a:t>𝑏𝑡</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
@@ -6721,7 +6721,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4457700" y="10034270"/>
+          <a:off x="4505325" y="10034270"/>
           <a:ext cx="506730" cy="192405"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6891,7 +6891,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5367020" y="10261600"/>
+          <a:off x="5414645" y="10261600"/>
           <a:ext cx="497840" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7059,7 +7059,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6406515" y="9310370"/>
+          <a:off x="6454140" y="9310370"/>
           <a:ext cx="582930" cy="360680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7229,7 +7229,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1926590" y="488315"/>
+          <a:off x="1974215" y="488315"/>
           <a:ext cx="6928485" cy="725170"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -7394,7 +7394,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9755505" y="1231265"/>
+          <a:off x="9803130" y="1231265"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7444,7 +7444,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10396220" y="1226820"/>
+          <a:off x="10443845" y="1226820"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7494,7 +7494,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6648450" y="1216660"/>
+          <a:off x="6696075" y="1216660"/>
           <a:ext cx="3175" cy="477520"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7544,7 +7544,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2898140" y="1229360"/>
+          <a:off x="2945765" y="1229360"/>
           <a:ext cx="3175" cy="477520"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7594,7 +7594,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true">
-          <a:off x="9755505" y="2356485"/>
+          <a:off x="9803130" y="2356485"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7644,7 +7644,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true">
-          <a:off x="10396220" y="2369185"/>
+          <a:off x="10443845" y="2369185"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7694,7 +7694,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3562350" y="5226685"/>
+          <a:off x="3609975" y="5226685"/>
           <a:ext cx="8890" cy="394970"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7744,7 +7744,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true">
-          <a:off x="7123430" y="5227955"/>
+          <a:off x="7171055" y="5227955"/>
           <a:ext cx="5080" cy="370205"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7777,13 +7777,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>452755</xdr:colOff>
+      <xdr:colOff>452120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>262890</xdr:rowOff>
+      <xdr:rowOff>262255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3154680</xdr:colOff>
+      <xdr:colOff>3326765</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1058545</xdr:rowOff>
     </xdr:to>
@@ -7796,8 +7796,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2190750" y="5634990"/>
-              <a:ext cx="2701925" cy="2294255"/>
+              <a:off x="2237740" y="5634355"/>
+              <a:ext cx="2874645" cy="2294890"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst/>
@@ -8038,8 +8038,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2190750" y="5634990"/>
-              <a:ext cx="2701925" cy="2294255"/>
+              <a:off x="2237740" y="5634355"/>
+              <a:ext cx="2874645" cy="2294890"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst/>
@@ -8278,7 +8278,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3764280" y="8331200"/>
+          <a:off x="3811905" y="8331200"/>
           <a:ext cx="2623185" cy="1766570"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -8437,7 +8437,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2060575" y="10423525"/>
+          <a:off x="2108200" y="10423525"/>
           <a:ext cx="6019165" cy="905510"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -8599,7 +8599,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true">
-          <a:off x="5073650" y="10097135"/>
+          <a:off x="5121275" y="10097135"/>
           <a:ext cx="5715" cy="326390"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -8649,7 +8649,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11106150" y="1226820"/>
+          <a:off x="11153775" y="1226820"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -8699,7 +8699,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true">
-          <a:off x="11106150" y="2369185"/>
+          <a:off x="11153775" y="2369185"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -8749,7 +8749,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11816080" y="1226820"/>
+          <a:off x="11863705" y="1226820"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -8799,7 +8799,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true">
-          <a:off x="11816080" y="2369185"/>
+          <a:off x="11863705" y="2369185"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -8832,13 +8832,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1803717</xdr:colOff>
+      <xdr:colOff>1888807</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1058227</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3341052</xdr:colOff>
+      <xdr:colOff>3337242</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>227647</xdr:rowOff>
     </xdr:to>
@@ -8852,12 +8852,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipV="true">
-          <a:off x="4109085" y="7360285"/>
-          <a:ext cx="401320" cy="1537335"/>
+          <a:off x="4197350" y="7404735"/>
+          <a:ext cx="401320" cy="1448435"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 28333"/>
+            <a:gd name="adj1" fmla="val 38968"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -8887,13 +8887,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3341370</xdr:colOff>
+      <xdr:colOff>3337560</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1000125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1654810</xdr:colOff>
+      <xdr:colOff>1715770</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>227965</xdr:rowOff>
     </xdr:to>
@@ -8907,12 +8907,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="5833110" y="7117080"/>
-          <a:ext cx="459740" cy="1967230"/>
+          <a:off x="5909310" y="7084695"/>
+          <a:ext cx="459740" cy="2032000"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 37465"/>
+            <a:gd name="adj1" fmla="val 46883"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="38100">
@@ -8961,7 +8961,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2014220" y="1699260"/>
+              <a:off x="2061845" y="1699260"/>
               <a:ext cx="6750685" cy="3495040"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
@@ -9293,7 +9293,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2014220" y="1699260"/>
+              <a:off x="2061845" y="1699260"/>
               <a:ext cx="6750685" cy="3495040"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
@@ -9578,11 +9578,11 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>205105</xdr:rowOff>
+      <xdr:rowOff>203835</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3006090</xdr:colOff>
+      <xdr:colOff>3126105</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1000125</xdr:rowOff>
     </xdr:to>
@@ -9595,8 +9595,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5696585" y="5577205"/>
-              <a:ext cx="2701290" cy="2293620"/>
+              <a:off x="5744210" y="5575935"/>
+              <a:ext cx="2821305" cy="2294890"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst/>
@@ -9740,7 +9740,7 @@
                 <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
                   <a:sym typeface="+mn-ea"/>
                 </a:rPr>
-                <a:t>Ranqueia os pares para cada variável de acordo com o </a:t>
+                <a:t>Para cada variável, eanqueia os pares de acordo com o </a:t>
               </a:r>
               <a14:m>
                 <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
@@ -9845,8 +9845,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5696585" y="5577205"/>
-              <a:ext cx="2701290" cy="2293620"/>
+              <a:off x="5744210" y="5575935"/>
+              <a:ext cx="2821305" cy="2294890"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst/>
@@ -9990,7 +9990,7 @@
                 <a:rPr lang="pt-PT" altLang="en-US" sz="1600">
                   <a:sym typeface="+mn-ea"/>
                 </a:rPr>
-                <a:t>Ranqueia os pares para cada variável de acordo com o </a:t>
+                <a:t>Para cada variável, eanqueia os pares de acordo com o </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" altLang="pt-PT" sz="1600">
@@ -10096,7 +10096,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="true" flipV="true">
-          <a:off x="5393055" y="1699260"/>
+          <a:off x="5440680" y="1699260"/>
           <a:ext cx="993775" cy="7515225"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
@@ -24694,13 +24694,13 @@
   <sheetPr/>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="22.8083333333333" customWidth="true"/>
+    <col min="1" max="1" width="23.4333333333333" customWidth="true"/>
     <col min="2" max="2" width="47.95" customWidth="true"/>
     <col min="3" max="3" width="48.8583333333333" customWidth="true"/>
     <col min="4" max="5" width="8.40833333333333" customWidth="true"/>
@@ -25013,7 +25013,7 @@
   <sheetPr/>
   <dimension ref="B1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>